<commit_message>
close review points from 1 to 3
</commit_message>
<xml_diff>
--- a/input_documents/CR/Review/PO_SB_CR_ML_Review.xlsx
+++ b/input_documents/CR/Review/PO_SB_CR_ML_Review.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Entry Date</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>All tables and headers shall be aligned together</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="8">
     <dxf>
       <font>
         <b/>
@@ -211,29 +214,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF57BB8A"/>
           <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -280,75 +260,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF57BB8A"/>
           <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF57BB8A"/>
-          <bgColor rgb="FF57BB8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -602,8 +513,8 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -665,7 +576,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -691,7 +602,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -717,7 +628,7 @@
         <v>20</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -783,42 +694,42 @@
     <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A5:H9">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>$H5 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:H9">
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>$H5= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:H2 A3">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:H2 A3">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:H3">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$H3 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:H3">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$H3= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:H4">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$H4 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:H4">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$H4= "Open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>